<commit_message>
allow sending of certificates with mail
</commit_message>
<xml_diff>
--- a/data/Bewertungen.xlsx
+++ b/data/Bewertungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tburakonat/TechAcademy/certificates-script/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC91231-D549-DF4E-8E34-EEE24DAB6B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34479592-603A-9542-AC1C-4FFC9969DCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Vorname</t>
   </si>
@@ -101,13 +101,19 @@
   </si>
   <si>
     <t>[ING Bank]</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>burak.onat@tech-academy.io</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +125,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,14 +155,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -444,7 +461,7 @@
     <col min="7" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +477,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -477,8 +497,11 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -494,8 +517,11 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -511,8 +537,11 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -528,9 +557,16 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{AF2E132D-A55E-A649-A7D6-6E0835E5AB5D}"/>
+    <hyperlink ref="F3:F5" r:id="rId2" display="burak.onat@tech-academy.io" xr:uid="{B52BEECB-42D9-AA46-99AE-8A81457AC47F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add comment generation functionality
</commit_message>
<xml_diff>
--- a/data/Bewertungen.xlsx
+++ b/data/Bewertungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tburakonat/TechAcademy/certificates-script/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34479592-603A-9542-AC1C-4FFC9969DCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF95DD1-F9F8-6E44-8EBF-78181183484E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Vorname</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>burak.onat@tech-academy.io</t>
+  </si>
+  <si>
+    <t>Kommentar des Mentors</t>
+  </si>
+  <si>
+    <t>Hallo Burak, deine Abgabe war sehr gut!</t>
+  </si>
+  <si>
+    <t>Hallo Lionel, leider war deine Abgabe eine Katastrophe</t>
+  </si>
+  <si>
+    <t>Hallo Cristiano, deine Abgabe war ganz okay</t>
+  </si>
+  <si>
+    <t>Hallo lieber Anderson Talisca, sehr schönes Freistoßtor!</t>
   </si>
 </sst>
 </file>
@@ -444,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -458,10 +473,11 @@
     <col min="4" max="4" width="28.83203125" customWidth="1"/>
     <col min="5" max="5" width="31.83203125" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +496,11 @@
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -500,8 +519,11 @@
       <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -520,8 +542,11 @@
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -540,8 +565,11 @@
       <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -559,6 +587,9 @@
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>